<commit_message>
Added GERBER RS274X files for Varmo - Rev A1
</commit_message>
<xml_diff>
--- a/ArmazCape/Rev B2/doc/ArmazCape Pinout - Rev B2.xlsx
+++ b/ArmazCape/Rev B2/doc/ArmazCape Pinout - Rev B2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="150">
   <si>
     <t>ArmazCape Pinout</t>
   </si>
@@ -468,6 +468,12 @@
   </si>
   <si>
     <t>SW_EXT4</t>
+  </si>
+  <si>
+    <t>0x0c0</t>
+  </si>
+  <si>
+    <t>0x0c4</t>
   </si>
 </sst>
 </file>
@@ -517,16 +523,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -892,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,15 +910,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -962,58 +968,58 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
       <c r="K4" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
       <c r="K5" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="K6" t="s">
         <v>57</v>
       </c>
@@ -1023,12 +1029,12 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="K7" t="s">
         <v>58</v>
       </c>
@@ -1038,14 +1044,14 @@
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="K8" t="s">
         <v>59</v>
       </c>
@@ -1055,12 +1061,12 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="K9" t="s">
         <v>60</v>
       </c>
@@ -1070,14 +1076,14 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="K10" t="s">
         <v>61</v>
       </c>
@@ -1104,12 +1110,12 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="K11" t="s">
         <v>62</v>
       </c>
@@ -1595,14 +1601,14 @@
       <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
       <c r="K35" t="s">
         <v>86</v>
       </c>
@@ -1627,14 +1633,14 @@
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
       <c r="K37" t="s">
         <v>88</v>
       </c>
@@ -1671,6 +1677,9 @@
       <c r="K40" t="s">
         <v>91</v>
       </c>
+      <c r="L40" t="s">
+        <v>148</v>
+      </c>
       <c r="M40" t="s">
         <v>139</v>
       </c>
@@ -1695,6 +1704,9 @@
       <c r="K41" t="s">
         <v>92</v>
       </c>
+      <c r="L41" t="s">
+        <v>149</v>
+      </c>
       <c r="M41" t="s">
         <v>140</v>
       </c>
@@ -1757,14 +1769,14 @@
       <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
       <c r="K46" t="s">
         <v>97</v>
       </c>
@@ -1773,12 +1785,12 @@
       <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
       <c r="K47" t="s">
         <v>98</v>
       </c>
@@ -1787,12 +1799,12 @@
       <c r="A48" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
       <c r="K48" t="s">
         <v>99</v>
       </c>
@@ -1801,28 +1813,28 @@
       <c r="A49" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
       <c r="K49" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C8:H9"/>
+    <mergeCell ref="C10:H11"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C46:H49"/>
     <mergeCell ref="M4:R5"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="C6:H7"/>
-    <mergeCell ref="C8:H9"/>
-    <mergeCell ref="C10:H11"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="C46:H49"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576 N1:N1048576">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">

</xml_diff>